<commit_message>
Arreglo en Encuesta Casa - Abasto
</commit_message>
<xml_diff>
--- a/src/Pequiven/SEIPBundle/Resources/Skeleton/workStudyCircle/Cuestionario_Casa_Abasto.xlsx
+++ b/src/Pequiven/SEIPBundle/Resources/Skeleton/workStudyCircle/Cuestionario_Casa_Abasto.xlsx
@@ -46,84 +46,84 @@
     <t>1.- ¿Conoce Usted qué es la Casa Abasto?</t>
   </si>
   <si>
-    <t>2.- ¿Cómo valoraría que se haya organizado la última jornadas de Casa Abasto mediante los CETP?</t>
-  </si>
-  <si>
-    <t>3.- ¿Considera que los Precios Ofertados por cada Producto son Justos y Accesibles?</t>
-  </si>
-  <si>
-    <t>4.- ¿Está usted Dispuesto a Apoyar Activamente en la Organización y Logística de las Próximas Jornadas de Casa Abasto?</t>
-  </si>
-  <si>
-    <t>5.- ¿Usted conoce los mecanismos de distribución y producción de la Gran Misión Abastecimiento Seguro? Si su Respuesta es Si, Menciónelos</t>
-  </si>
-  <si>
-    <t>6.- ¿Usted Conoce para que se Organizan las Jornadas de Abastecimiento?
+    <t>MUY BUENA</t>
+  </si>
+  <si>
+    <t>BUENA</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>MALA</t>
+  </si>
+  <si>
+    <t>MUY MALA</t>
+  </si>
+  <si>
+    <t>7.- ¿Cómo Consideró Usted el Desarrollo de la Última Jornadas de Casa Abasto?</t>
+  </si>
+  <si>
+    <t>JUSTICIA</t>
+  </si>
+  <si>
+    <t>SOLIDARIDAD</t>
+  </si>
+  <si>
+    <t>COMPROMISO</t>
+  </si>
+  <si>
+    <t>IGUALDAD</t>
+  </si>
+  <si>
+    <t>OTROS</t>
+  </si>
+  <si>
+    <t>8.- ¿Qué Valores Socialistas se Fomentan Mediante este Tipo de Jornadas?</t>
+  </si>
+  <si>
+    <t>b. OPINE SOBRE LAS SIGUIENTES PREGUNTAS</t>
+  </si>
+  <si>
+    <t>OPINE</t>
+  </si>
+  <si>
+    <t>9.- ¿Usted Conoce Cuál es el Origen del Desabastecimiento del País?</t>
+  </si>
+  <si>
+    <t>10.- ¿Este Tipo de Jornadas Contribuyen a Derrotar la Guerra Económica impuesta al Pueblo Venezolano?</t>
+  </si>
+  <si>
+    <t>11.- ¿Tiene Alguna Recomendación o Sugerencia Referente a la Última Jornada de Casa Abasto?</t>
+  </si>
+  <si>
+    <t>IdUser</t>
+  </si>
+  <si>
+    <t>IdWSC</t>
+  </si>
+  <si>
+    <t>2.- ¿Considera que los Precios Ofertados por cada Producto son Justos y Accesibles?</t>
+  </si>
+  <si>
+    <t>3.- ¿Está usted Dispuesto a Apoyar Activamente en la Organización y Logística de las Próximas Jornadas de Casa Abasto?</t>
+  </si>
+  <si>
+    <t>4.- ¿Usted conoce los mecanismos de distribución y producción de la Gran Misión Abastecimiento Seguro? Si su Respuesta es Si, Menciónelos</t>
+  </si>
+  <si>
+    <t>5.- ¿Usted Conoce para que se Organizan las Jornadas de Abastecimiento?
 Si su Respuesta es Si, Menciónelos</t>
   </si>
   <si>
-    <t>MUY BUENA</t>
-  </si>
-  <si>
-    <t>BUENA</t>
-  </si>
-  <si>
-    <t>REGULAR</t>
-  </si>
-  <si>
-    <t>MALA</t>
-  </si>
-  <si>
-    <t>MUY MALA</t>
-  </si>
-  <si>
-    <t>7.- ¿Cómo Consideró Usted el Desarrollo de la Última Jornadas de Casa Abasto?</t>
-  </si>
-  <si>
-    <t>JUSTICIA</t>
-  </si>
-  <si>
-    <t>SOLIDARIDAD</t>
-  </si>
-  <si>
-    <t>COMPROMISO</t>
-  </si>
-  <si>
-    <t>IGUALDAD</t>
-  </si>
-  <si>
-    <t>OTROS</t>
-  </si>
-  <si>
-    <t>8.- ¿Qué Valores Socialistas se Fomentan Mediante este Tipo de Jornadas?</t>
-  </si>
-  <si>
-    <t>b. OPINE SOBRE LAS SIGUIENTES PREGUNTAS</t>
-  </si>
-  <si>
-    <t>OPINE</t>
-  </si>
-  <si>
-    <t>9.- ¿Usted Conoce Cuál es el Origen del Desabastecimiento del País?</t>
-  </si>
-  <si>
-    <t>10.- ¿Este Tipo de Jornadas Contribuyen a Derrotar la Guerra Económica impuesta al Pueblo Venezolano?</t>
-  </si>
-  <si>
-    <t>11.- ¿Tiene Alguna Recomendación o Sugerencia Referente a la Última Jornada de Casa Abasto?</t>
-  </si>
-  <si>
-    <t>IdUser</t>
-  </si>
-  <si>
-    <t>IdWSC</t>
+    <t>6.- ¿Cómo valoraría que se haya organizado la última jornadas de Casa Abasto mediante los CETP?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,12 +171,6 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Liberation Sans Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <name val="Liberation Sans Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -244,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -537,19 +531,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -603,18 +584,149 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -650,13 +762,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -671,12 +783,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,154 +792,42 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -841,8 +835,159 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1299,369 +1444,369 @@
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="109.140625" style="2"/>
-    <col min="2" max="3" width="21.7109375" style="3"/>
-    <col min="4" max="4" width="22.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="21.7109375" style="3"/>
-    <col min="7" max="1022" width="11.5703125" style="2"/>
-    <col min="1023" max="1025" width="11.5703125" style="4"/>
+    <col min="1" max="1" width="109.140625" style="1"/>
+    <col min="2" max="3" width="21.7109375" style="2"/>
+    <col min="4" max="4" width="22.85546875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="21.7109375" style="2"/>
+    <col min="7" max="1022" width="11.5703125" style="1"/>
+    <col min="1023" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="2" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="3" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="4" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="5" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="6" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="7" spans="1:1024" s="4" customFormat="1" ht="12.75"/>
-    <row r="8" spans="1:1024" s="4" customFormat="1" ht="39.75" customHeight="1"/>
-    <row r="9" spans="1:1024" s="4" customFormat="1" ht="12.75">
-      <c r="A9" s="1" t="s">
+    <row r="1" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="2" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="3" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="4" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="5" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="6" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="7" spans="1:1024" s="3" customFormat="1" ht="12.75"/>
+    <row r="8" spans="1:1024" s="3" customFormat="1" ht="39.75" customHeight="1"/>
+    <row r="9" spans="1:1024" s="3" customFormat="1" ht="12.75">
+      <c r="A9" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:1024" s="4" customFormat="1" ht="12.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:1024" s="4" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="12" spans="1:1024" s="5" customFormat="1" ht="28.35" customHeight="1">
-      <c r="B12" s="19" t="s">
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+    </row>
+    <row r="10" spans="1:1024" s="3" customFormat="1" ht="12.75">
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+    </row>
+    <row r="11" spans="1:1024" s="3" customFormat="1" ht="13.5" thickBot="1"/>
+    <row r="12" spans="1:1024" s="4" customFormat="1" ht="28.35" customHeight="1">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="AMI12" s="6"/>
-      <c r="AMJ12" s="6"/>
-    </row>
-    <row r="13" spans="1:1024" s="5" customFormat="1" ht="28.35" customHeight="1" thickBot="1">
-      <c r="B13" s="24" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="AMI12" s="5"/>
+      <c r="AMJ12" s="5"/>
+    </row>
+    <row r="13" spans="1:1024" s="4" customFormat="1" ht="28.35" customHeight="1" thickBot="1">
+      <c r="B13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="AMI13" s="6"/>
-      <c r="AMJ13" s="6"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="AMI13" s="5"/>
+      <c r="AMJ13" s="5"/>
     </row>
     <row r="14" spans="1:1024" ht="21" thickBot="1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:1024" ht="17.45" customHeight="1" thickBot="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:1024" ht="36.950000000000003" customHeight="1">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="36.950000000000003" customHeight="1">
+      <c r="A18" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" ht="36.950000000000003" customHeight="1">
+      <c r="A19" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A20" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A22" s="11"/>
+      <c r="B22" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A18" s="38" t="s">
+      <c r="C22" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A19" s="38" t="s">
+      <c r="D22" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A20" s="38" t="s">
+      <c r="E22" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
-      <c r="A21" s="39" t="s">
+      <c r="F22" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A24" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="C25" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="D25" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="E25" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
-      <c r="A24" s="54" t="s">
+      <c r="F25" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="36.950000000000003" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="55" t="s">
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
+      <c r="A26" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="7"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="21" thickBot="1">
+      <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" ht="18.75" thickBot="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="45"/>
+    </row>
+    <row r="31" spans="1:9" ht="57" customHeight="1">
+      <c r="A31" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="57" t="s">
+      <c r="B31" s="46"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="48"/>
+    </row>
+    <row r="32" spans="1:9" ht="57" customHeight="1">
+      <c r="A32" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="36.950000000000003" customHeight="1" thickBot="1">
-      <c r="A26" s="54" t="s">
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="51"/>
+    </row>
+    <row r="33" spans="1:6" ht="57" customHeight="1" thickBot="1">
+      <c r="A33" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="8"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="8"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" ht="21" thickBot="1">
-      <c r="A29" s="7" t="s">
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+    </row>
+    <row r="34" spans="1:6" ht="18.95" customHeight="1">
+      <c r="A34" s="13"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" hidden="1">
+      <c r="A35" s="7"/>
+      <c r="C35" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-    </row>
-    <row r="30" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="64" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66"/>
-    </row>
-    <row r="31" spans="1:9" ht="57" customHeight="1">
-      <c r="A31" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
-    </row>
-    <row r="32" spans="1:9" ht="57" customHeight="1">
-      <c r="A32" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="59"/>
-    </row>
-    <row r="33" spans="1:6" ht="57" customHeight="1" thickBot="1">
-      <c r="A33" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
-    </row>
-    <row r="34" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="1:6" hidden="1">
-      <c r="A35" s="8"/>
-      <c r="C35" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F35" s="18"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" hidden="1"/>
   </sheetData>
-  <sheetProtection password="DCDA" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection password="DCDA" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="11">
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="D16:F18"/>
     <mergeCell ref="A9:F10"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F19"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.59027777777777801" right="0.59027777777777801" top="0.59027777777777801" bottom="0.59027777777777801" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup scale="58" orientation="landscape" useFirstPageNumber="1" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="58" orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="1" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>